<commit_message>
Semana 10: Sexto grado
</commit_message>
<xml_diff>
--- a/santillana-recursos/semana_10/LGS5_Aprende en casa_GAVI_Semana 10_2021-2022.xlsx
+++ b/santillana-recursos/semana_10/LGS5_Aprende en casa_GAVI_Semana 10_2021-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fceron/Desktop/APRENDE EN CASA/SEMANA 10/DEFINITIVOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos.ciddelapaz/Library/Mobile Documents/com~apple~CloudDocs/Dev/GitHub/gavi/santillana-recursos/semana_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0707A56-0BF4-EB42-B347-18B9083F8768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB64476-1850-D944-999D-9D5B2016113E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="460" windowWidth="35100" windowHeight="22120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 10" sheetId="4" r:id="rId1"/>
@@ -931,7 +931,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -978,15 +978,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -998,9 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1462,10 +1450,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1473,7 +1461,7 @@
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="8" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="20" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" style="9" customWidth="1"/>
     <col min="6" max="6" width="21.5" style="10" customWidth="1"/>
     <col min="7" max="7" width="23.5" style="1" customWidth="1"/>
@@ -1487,50 +1475,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="74"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
     </row>
     <row r="5" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1559,13 +1547,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -1585,11 +1573,11 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="76"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="72"/>
+      <c r="B7" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -1609,11 +1597,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="89" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="76"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -1633,11 +1621,11 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="76"/>
-      <c r="B9" s="34" t="s">
+      <c r="A9" s="72"/>
+      <c r="B9" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -1655,14 +1643,14 @@
       <c r="H9" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="58"/>
+      <c r="I9" s="54"/>
     </row>
     <row r="10" spans="1:9" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="77"/>
-      <c r="B10" s="34" t="s">
+      <c r="A10" s="73"/>
+      <c r="B10" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -1674,497 +1662,470 @@
       <c r="F10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="61" t="s">
+      <c r="G10" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="56"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
+      <c r="H10" s="52"/>
+    </row>
+    <row r="11" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B11" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>16</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="62"/>
+      <c r="B12" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="16" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66"/>
-      <c r="B13" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>17</v>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="1:9" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="62"/>
+      <c r="B13" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="59"/>
-    </row>
-    <row r="14" spans="1:9" ht="79" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="66"/>
-      <c r="B14" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="19" t="s">
+    </row>
+    <row r="14" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="62"/>
+      <c r="B14" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="77"/>
+      <c r="B15" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="37"/>
+      <c r="H15" s="36"/>
+    </row>
+    <row r="16" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="56"/>
+    </row>
+    <row r="17" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="62"/>
+      <c r="B17" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="62"/>
+      <c r="B18" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="62"/>
+      <c r="B19" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="77"/>
+      <c r="B20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="66"/>
-      <c r="B15" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="37" t="s">
+      <c r="E21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="75"/>
+      <c r="B22" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="75"/>
+      <c r="B23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I23" s="56"/>
+    </row>
+    <row r="24" spans="1:9" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="75"/>
+      <c r="B24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D24" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="76"/>
+      <c r="B25" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="62"/>
+      <c r="B27" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="81"/>
-      <c r="B16" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="39" t="s">
+      <c r="E27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="62"/>
+      <c r="B28" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="62"/>
+      <c r="B29" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="1:9" s="32" customFormat="1" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="63"/>
+      <c r="B30" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="40"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="60"/>
-    </row>
-    <row r="19" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="66"/>
-      <c r="B19" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="66"/>
-      <c r="B20" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="66"/>
-      <c r="B21" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="81"/>
-      <c r="B22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="79"/>
-      <c r="B25" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="79"/>
-      <c r="B26" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I26" s="60"/>
-    </row>
-    <row r="27" spans="1:9" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="79"/>
-      <c r="B27" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="80"/>
-      <c r="B28" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="30" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="65" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="66"/>
-      <c r="B31" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="66"/>
-      <c r="B32" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="1:8" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="66"/>
-      <c r="B33" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="51"/>
-    </row>
-    <row r="34" spans="1:8" s="36" customFormat="1" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="67"/>
-      <c r="B34" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="63" t="s">
+      <c r="D30" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E30" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F30" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G34" s="55" t="s">
+      <c r="G30" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="H34" s="57"/>
+      <c r="H30" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A26:A30"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>